<commit_message>
Abstract, introduction, fazit bearbeitet
</commit_message>
<xml_diff>
--- a/Auswertung-MR/Excel/JKopplung.xlsx
+++ b/Auswertung-MR/Excel/JKopplung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Dokumente\Studium\Konstanz\7. Semester\FP\EFNMR-Remote\Auswertung-MR\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA884ED-1449-44A3-BC23-30D415F0169A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E816A56-A8BF-48D0-96D3-69B8FF8D6330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2088" yWindow="1428" windowWidth="12084" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Fit Parameter</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Normierung</t>
+  </si>
+  <si>
+    <t>uc</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,8 +756,8 @@
         <v>0.55255292835604941</v>
       </c>
       <c r="V15">
-        <f>B18/B24</f>
-        <v>1.1904761904761905</v>
+        <f>B18/B18</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -791,8 +794,8 @@
         <v>0.76682987088992571</v>
       </c>
       <c r="V16">
-        <f>B21/B24</f>
-        <v>2.8571619047619046</v>
+        <f>B21/B18</f>
+        <v>2.4000159999999999</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
@@ -832,8 +835,8 @@
         <v>0.39050003325275567</v>
       </c>
       <c r="V17">
-        <f>B24/B24</f>
-        <v>1</v>
+        <f>B24/B18</f>
+        <v>0.84000000000000008</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -989,6 +992,29 @@
       <c r="I26">
         <f>I25/(2*PI())</f>
         <v>5.3697967391250385E-2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <f>AVERAGE(L21,L9)</f>
+        <v>6.3222279261226557</v>
+      </c>
+      <c r="O27">
+        <f>STDEV(L9,L21)/SQRT(2)</f>
+        <v>4.7771983425063169E-2</v>
+      </c>
+      <c r="P27">
+        <f>SQRT((M9)^2+(M21)^2)</f>
+        <v>1.3021497936611608</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f>110/(2*PI())</f>
+        <v>17.507043740108486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>